<commit_message>
* #7856 #7857 #7860 #7870
</commit_message>
<xml_diff>
--- a/storage/app/excel/contact_book_2.xlsx
+++ b/storage/app/excel/contact_book_2.xlsx
@@ -1,20 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\新しいフォルダー (2)\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B6A97E-FC18-410C-8311-06060AACC1A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12495"/>
+    <workbookView xWindow="2100" yWindow="1290" windowWidth="28410" windowHeight="14205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$Z$21</definedName>
+  </definedNames>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>001-保育園</t>
   </si>
@@ -25,9 +44,6 @@
     <t>天気</t>
   </si>
   <si>
-    <t>記入者 保護者様名</t>
-  </si>
-  <si>
     <t>保育士名</t>
   </si>
   <si>
@@ -36,178 +52,52 @@
   <si>
     <t>保育園からの連絡事項</t>
   </si>
+  <si>
+    <t>記入者</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>保護者様名</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="21">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -232,194 +122,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="16">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -506,16 +210,27 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color auto="1"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -523,349 +238,149 @@
       <left/>
       <right/>
       <top style="thin">
-        <color theme="4"/>
+        <color indexed="64"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="58" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+  <cellStyles count="1">
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1123,31 +638,42 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:AG55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:M17"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="60" zoomScaleSheetLayoutView="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="21" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="6.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.625" style="2" customWidth="1"/>
+    <col min="3" max="8" width="6.625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="12.625" style="2" customWidth="1"/>
+    <col min="10" max="17" width="6.625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="12.625" style="2" customWidth="1"/>
+    <col min="19" max="26" width="6.625" style="2" customWidth="1"/>
+    <col min="27" max="16384" width="9.125" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:33" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1"/>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
@@ -1174,15 +700,15 @@
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
     </row>
-    <row r="2" spans="1:33">
+    <row r="2" spans="1:33" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -1209,7 +735,7 @@
       <c r="AF2" s="1"/>
       <c r="AG2" s="1"/>
     </row>
-    <row r="3" spans="1:33">
+    <row r="3" spans="1:33" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1244,39 +770,39 @@
       <c r="AF3" s="1"/>
       <c r="AG3" s="1"/>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:33" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1"/>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="18">
         <v>44598</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="5" t="s">
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
-      <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="22"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
       <c r="AA4" s="1"/>
       <c r="AB4" s="1"/>
       <c r="AC4" s="1"/>
@@ -1285,33 +811,33 @@
       <c r="AF4" s="1"/>
       <c r="AG4" s="1"/>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:33" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
       <c r="AA5" s="1"/>
       <c r="AB5" s="1"/>
       <c r="AC5" s="1"/>
@@ -1320,37 +846,39 @@
       <c r="AF5" s="1"/>
       <c r="AG5" s="1"/>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:33" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1"/>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="22"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="5"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
       <c r="AA6" s="1"/>
       <c r="AB6" s="1"/>
       <c r="AC6" s="1"/>
@@ -1359,33 +887,33 @@
       <c r="AF6" s="1"/>
       <c r="AG6" s="1"/>
     </row>
-    <row r="7" spans="1:33">
+    <row r="7" spans="1:33" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
-      <c r="W7" s="1"/>
-      <c r="X7" s="1"/>
-      <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
       <c r="AA7" s="1"/>
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
@@ -1394,33 +922,33 @@
       <c r="AF7" s="1"/>
       <c r="AG7" s="1"/>
     </row>
-    <row r="8" spans="1:33">
+    <row r="8" spans="1:33" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
-      <c r="W8" s="1"/>
-      <c r="X8" s="1"/>
-      <c r="Y8" s="1"/>
-      <c r="Z8" s="1"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
       <c r="AA8" s="1"/>
       <c r="AB8" s="1"/>
       <c r="AC8" s="1"/>
@@ -1429,10 +957,10 @@
       <c r="AF8" s="1"/>
       <c r="AG8" s="1"/>
     </row>
-    <row r="9" spans="1:33">
+    <row r="9" spans="1:33" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1"/>
       <c r="B9" s="6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -1444,9 +972,9 @@
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
-      <c r="M9" s="11"/>
+      <c r="M9" s="8"/>
       <c r="N9" s="12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O9" s="13"/>
       <c r="P9" s="13"/>
@@ -1458,8 +986,8 @@
       <c r="V9" s="13"/>
       <c r="W9" s="13"/>
       <c r="X9" s="13"/>
-      <c r="Y9" s="17"/>
-      <c r="Z9" s="1"/>
+      <c r="Y9" s="14"/>
+      <c r="Z9" s="3"/>
       <c r="AA9" s="1"/>
       <c r="AB9" s="1"/>
       <c r="AC9" s="1"/>
@@ -1468,20 +996,20 @@
       <c r="AF9" s="1"/>
       <c r="AG9" s="1"/>
     </row>
-    <row r="10" spans="1:33">
+    <row r="10" spans="1:33" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="14"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="11"/>
       <c r="N10" s="15"/>
       <c r="O10" s="16"/>
       <c r="P10" s="16"/>
@@ -1493,8 +1021,8 @@
       <c r="V10" s="16"/>
       <c r="W10" s="16"/>
       <c r="X10" s="16"/>
-      <c r="Y10" s="18"/>
-      <c r="Z10" s="1"/>
+      <c r="Y10" s="17"/>
+      <c r="Z10" s="3"/>
       <c r="AA10" s="1"/>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
@@ -1503,33 +1031,33 @@
       <c r="AF10" s="1"/>
       <c r="AG10" s="1"/>
     </row>
-    <row r="11" spans="1:33">
+    <row r="11" spans="1:33" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="10"/>
-      <c r="R11" s="10"/>
-      <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
-      <c r="U11" s="10"/>
-      <c r="V11" s="10"/>
-      <c r="W11" s="10"/>
-      <c r="X11" s="10"/>
-      <c r="Y11" s="10"/>
-      <c r="Z11" s="1"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="25"/>
+      <c r="Q11" s="25"/>
+      <c r="R11" s="25"/>
+      <c r="S11" s="25"/>
+      <c r="T11" s="25"/>
+      <c r="U11" s="25"/>
+      <c r="V11" s="25"/>
+      <c r="W11" s="25"/>
+      <c r="X11" s="25"/>
+      <c r="Y11" s="26"/>
+      <c r="Z11" s="3"/>
       <c r="AA11" s="1"/>
       <c r="AB11" s="1"/>
       <c r="AC11" s="1"/>
@@ -1538,33 +1066,33 @@
       <c r="AF11" s="1"/>
       <c r="AG11" s="1"/>
     </row>
-    <row r="12" spans="1:33">
+    <row r="12" spans="1:33" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="10"/>
-      <c r="R12" s="10"/>
-      <c r="S12" s="10"/>
-      <c r="T12" s="10"/>
-      <c r="U12" s="10"/>
-      <c r="V12" s="10"/>
-      <c r="W12" s="10"/>
-      <c r="X12" s="10"/>
-      <c r="Y12" s="10"/>
-      <c r="Z12" s="1"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="28"/>
+      <c r="P12" s="28"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="28"/>
+      <c r="S12" s="28"/>
+      <c r="T12" s="28"/>
+      <c r="U12" s="28"/>
+      <c r="V12" s="28"/>
+      <c r="W12" s="28"/>
+      <c r="X12" s="28"/>
+      <c r="Y12" s="29"/>
+      <c r="Z12" s="3"/>
       <c r="AA12" s="1"/>
       <c r="AB12" s="1"/>
       <c r="AC12" s="1"/>
@@ -1573,33 +1101,33 @@
       <c r="AF12" s="1"/>
       <c r="AG12" s="1"/>
     </row>
-    <row r="13" spans="1:33">
+    <row r="13" spans="1:33" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="10"/>
-      <c r="S13" s="10"/>
-      <c r="T13" s="10"/>
-      <c r="U13" s="10"/>
-      <c r="V13" s="10"/>
-      <c r="W13" s="10"/>
-      <c r="X13" s="10"/>
-      <c r="Y13" s="10"/>
-      <c r="Z13" s="1"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="28"/>
+      <c r="R13" s="28"/>
+      <c r="S13" s="28"/>
+      <c r="T13" s="28"/>
+      <c r="U13" s="28"/>
+      <c r="V13" s="28"/>
+      <c r="W13" s="28"/>
+      <c r="X13" s="28"/>
+      <c r="Y13" s="29"/>
+      <c r="Z13" s="3"/>
       <c r="AA13" s="1"/>
       <c r="AB13" s="1"/>
       <c r="AC13" s="1"/>
@@ -1608,33 +1136,33 @@
       <c r="AF13" s="1"/>
       <c r="AG13" s="1"/>
     </row>
-    <row r="14" spans="1:33">
+    <row r="14" spans="1:33" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="10"/>
-      <c r="V14" s="10"/>
-      <c r="W14" s="10"/>
-      <c r="X14" s="10"/>
-      <c r="Y14" s="10"/>
-      <c r="Z14" s="1"/>
+      <c r="B14" s="27"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="27"/>
+      <c r="O14" s="28"/>
+      <c r="P14" s="28"/>
+      <c r="Q14" s="28"/>
+      <c r="R14" s="28"/>
+      <c r="S14" s="28"/>
+      <c r="T14" s="28"/>
+      <c r="U14" s="28"/>
+      <c r="V14" s="28"/>
+      <c r="W14" s="28"/>
+      <c r="X14" s="28"/>
+      <c r="Y14" s="29"/>
+      <c r="Z14" s="3"/>
       <c r="AA14" s="1"/>
       <c r="AB14" s="1"/>
       <c r="AC14" s="1"/>
@@ -1643,33 +1171,33 @@
       <c r="AF14" s="1"/>
       <c r="AG14" s="1"/>
     </row>
-    <row r="15" spans="1:33">
+    <row r="15" spans="1:33" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
-      <c r="U15" s="10"/>
-      <c r="V15" s="10"/>
-      <c r="W15" s="10"/>
-      <c r="X15" s="10"/>
-      <c r="Y15" s="10"/>
-      <c r="Z15" s="1"/>
+      <c r="B15" s="27"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="27"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="28"/>
+      <c r="Q15" s="28"/>
+      <c r="R15" s="28"/>
+      <c r="S15" s="28"/>
+      <c r="T15" s="28"/>
+      <c r="U15" s="28"/>
+      <c r="V15" s="28"/>
+      <c r="W15" s="28"/>
+      <c r="X15" s="28"/>
+      <c r="Y15" s="29"/>
+      <c r="Z15" s="3"/>
       <c r="AA15" s="1"/>
       <c r="AB15" s="1"/>
       <c r="AC15" s="1"/>
@@ -1678,33 +1206,33 @@
       <c r="AF15" s="1"/>
       <c r="AG15" s="1"/>
     </row>
-    <row r="16" spans="1:33">
+    <row r="16" spans="1:33" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10"/>
-      <c r="U16" s="10"/>
-      <c r="V16" s="10"/>
-      <c r="W16" s="10"/>
-      <c r="X16" s="10"/>
-      <c r="Y16" s="10"/>
-      <c r="Z16" s="1"/>
+      <c r="B16" s="27"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="28"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="28"/>
+      <c r="Q16" s="28"/>
+      <c r="R16" s="28"/>
+      <c r="S16" s="28"/>
+      <c r="T16" s="28"/>
+      <c r="U16" s="28"/>
+      <c r="V16" s="28"/>
+      <c r="W16" s="28"/>
+      <c r="X16" s="28"/>
+      <c r="Y16" s="29"/>
+      <c r="Z16" s="3"/>
       <c r="AA16" s="1"/>
       <c r="AB16" s="1"/>
       <c r="AC16" s="1"/>
@@ -1713,33 +1241,33 @@
       <c r="AF16" s="1"/>
       <c r="AG16" s="1"/>
     </row>
-    <row r="17" spans="1:33">
+    <row r="17" spans="1:33" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="10"/>
-      <c r="S17" s="10"/>
-      <c r="T17" s="10"/>
-      <c r="U17" s="10"/>
-      <c r="V17" s="10"/>
-      <c r="W17" s="10"/>
-      <c r="X17" s="10"/>
-      <c r="Y17" s="10"/>
-      <c r="Z17" s="1"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="27"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="28"/>
+      <c r="Q17" s="28"/>
+      <c r="R17" s="28"/>
+      <c r="S17" s="28"/>
+      <c r="T17" s="28"/>
+      <c r="U17" s="28"/>
+      <c r="V17" s="28"/>
+      <c r="W17" s="28"/>
+      <c r="X17" s="28"/>
+      <c r="Y17" s="29"/>
+      <c r="Z17" s="3"/>
       <c r="AA17" s="1"/>
       <c r="AB17" s="1"/>
       <c r="AC17" s="1"/>
@@ -1748,33 +1276,33 @@
       <c r="AF17" s="1"/>
       <c r="AG17" s="1"/>
     </row>
-    <row r="18" spans="1:33">
+    <row r="18" spans="1:33" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
-      <c r="Q18" s="1"/>
-      <c r="R18" s="1"/>
-      <c r="S18" s="1"/>
-      <c r="T18" s="1"/>
-      <c r="U18" s="1"/>
-      <c r="V18" s="1"/>
-      <c r="W18" s="1"/>
-      <c r="X18" s="1"/>
-      <c r="Y18" s="1"/>
-      <c r="Z18" s="1"/>
+      <c r="B18" s="27"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="27"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28"/>
+      <c r="Q18" s="28"/>
+      <c r="R18" s="28"/>
+      <c r="S18" s="28"/>
+      <c r="T18" s="28"/>
+      <c r="U18" s="28"/>
+      <c r="V18" s="28"/>
+      <c r="W18" s="28"/>
+      <c r="X18" s="28"/>
+      <c r="Y18" s="29"/>
+      <c r="Z18" s="3"/>
       <c r="AA18" s="1"/>
       <c r="AB18" s="1"/>
       <c r="AC18" s="1"/>
@@ -1783,33 +1311,33 @@
       <c r="AF18" s="1"/>
       <c r="AG18" s="1"/>
     </row>
-    <row r="19" spans="1:33">
+    <row r="19" spans="1:33" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
-      <c r="Q19" s="1"/>
-      <c r="R19" s="1"/>
-      <c r="S19" s="1"/>
-      <c r="T19" s="1"/>
-      <c r="U19" s="1"/>
-      <c r="V19" s="1"/>
-      <c r="W19" s="1"/>
-      <c r="X19" s="1"/>
-      <c r="Y19" s="1"/>
-      <c r="Z19" s="1"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
+      <c r="L19" s="31"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="30"/>
+      <c r="O19" s="31"/>
+      <c r="P19" s="31"/>
+      <c r="Q19" s="31"/>
+      <c r="R19" s="31"/>
+      <c r="S19" s="31"/>
+      <c r="T19" s="31"/>
+      <c r="U19" s="31"/>
+      <c r="V19" s="31"/>
+      <c r="W19" s="31"/>
+      <c r="X19" s="31"/>
+      <c r="Y19" s="32"/>
+      <c r="Z19" s="3"/>
       <c r="AA19" s="1"/>
       <c r="AB19" s="1"/>
       <c r="AC19" s="1"/>
@@ -1818,33 +1346,33 @@
       <c r="AF19" s="1"/>
       <c r="AG19" s="1"/>
     </row>
-    <row r="20" spans="1:33">
+    <row r="20" spans="1:33" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
-      <c r="U20" s="1"/>
-      <c r="V20" s="1"/>
-      <c r="W20" s="1"/>
-      <c r="X20" s="1"/>
-      <c r="Y20" s="1"/>
-      <c r="Z20" s="1"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="3"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+      <c r="V20" s="3"/>
+      <c r="W20" s="3"/>
+      <c r="X20" s="3"/>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="3"/>
       <c r="AA20" s="1"/>
       <c r="AB20" s="1"/>
       <c r="AC20" s="1"/>
@@ -1853,33 +1381,33 @@
       <c r="AF20" s="1"/>
       <c r="AG20" s="1"/>
     </row>
-    <row r="21" spans="1:33">
+    <row r="21" spans="1:33" ht="27" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-      <c r="T21" s="1"/>
-      <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
-      <c r="W21" s="1"/>
-      <c r="X21" s="1"/>
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="1"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+      <c r="V21" s="3"/>
+      <c r="W21" s="3"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="3"/>
+      <c r="Z21" s="3"/>
       <c r="AA21" s="1"/>
       <c r="AB21" s="1"/>
       <c r="AC21" s="1"/>
@@ -1888,7 +1416,7 @@
       <c r="AF21" s="1"/>
       <c r="AG21" s="1"/>
     </row>
-    <row r="22" spans="1:33">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1923,7 +1451,7 @@
       <c r="AF22" s="1"/>
       <c r="AG22" s="1"/>
     </row>
-    <row r="23" spans="1:33">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1958,7 +1486,7 @@
       <c r="AF23" s="1"/>
       <c r="AG23" s="1"/>
     </row>
-    <row r="24" spans="1:33">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1993,7 +1521,7 @@
       <c r="AF24" s="1"/>
       <c r="AG24" s="1"/>
     </row>
-    <row r="25" spans="1:33">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2028,7 +1556,7 @@
       <c r="AF25" s="1"/>
       <c r="AG25" s="1"/>
     </row>
-    <row r="26" spans="1:33">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2063,7 +1591,7 @@
       <c r="AF26" s="1"/>
       <c r="AG26" s="1"/>
     </row>
-    <row r="27" spans="1:33">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -2098,7 +1626,7 @@
       <c r="AF27" s="1"/>
       <c r="AG27" s="1"/>
     </row>
-    <row r="28" spans="1:33">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -2133,7 +1661,7 @@
       <c r="AF28" s="1"/>
       <c r="AG28" s="1"/>
     </row>
-    <row r="29" spans="1:33">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -2168,7 +1696,7 @@
       <c r="AF29" s="1"/>
       <c r="AG29" s="1"/>
     </row>
-    <row r="30" spans="1:33">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -2203,7 +1731,7 @@
       <c r="AF30" s="1"/>
       <c r="AG30" s="1"/>
     </row>
-    <row r="31" spans="1:33">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -2238,7 +1766,7 @@
       <c r="AF31" s="1"/>
       <c r="AG31" s="1"/>
     </row>
-    <row r="32" spans="1:33">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -2273,7 +1801,7 @@
       <c r="AF32" s="1"/>
       <c r="AG32" s="1"/>
     </row>
-    <row r="33" spans="1:33">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -2308,7 +1836,7 @@
       <c r="AF33" s="1"/>
       <c r="AG33" s="1"/>
     </row>
-    <row r="34" spans="1:33">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -2343,7 +1871,7 @@
       <c r="AF34" s="1"/>
       <c r="AG34" s="1"/>
     </row>
-    <row r="35" spans="1:33">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -2378,7 +1906,7 @@
       <c r="AF35" s="1"/>
       <c r="AG35" s="1"/>
     </row>
-    <row r="36" spans="1:33">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -2413,7 +1941,7 @@
       <c r="AF36" s="1"/>
       <c r="AG36" s="1"/>
     </row>
-    <row r="37" spans="1:33">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -2448,7 +1976,7 @@
       <c r="AF37" s="1"/>
       <c r="AG37" s="1"/>
     </row>
-    <row r="38" spans="1:33">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -2483,7 +2011,7 @@
       <c r="AF38" s="1"/>
       <c r="AG38" s="1"/>
     </row>
-    <row r="39" spans="1:33">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -2518,7 +2046,7 @@
       <c r="AF39" s="1"/>
       <c r="AG39" s="1"/>
     </row>
-    <row r="40" spans="1:33">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -2553,7 +2081,7 @@
       <c r="AF40" s="1"/>
       <c r="AG40" s="1"/>
     </row>
-    <row r="41" spans="1:33">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -2588,7 +2116,7 @@
       <c r="AF41" s="1"/>
       <c r="AG41" s="1"/>
     </row>
-    <row r="42" spans="1:33">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -2623,7 +2151,7 @@
       <c r="AF42" s="1"/>
       <c r="AG42" s="1"/>
     </row>
-    <row r="43" spans="1:33">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -2658,7 +2186,7 @@
       <c r="AF43" s="1"/>
       <c r="AG43" s="1"/>
     </row>
-    <row r="44" spans="1:33">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -2693,7 +2221,7 @@
       <c r="AF44" s="1"/>
       <c r="AG44" s="1"/>
     </row>
-    <row r="45" spans="1:33">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -2728,7 +2256,7 @@
       <c r="AF45" s="1"/>
       <c r="AG45" s="1"/>
     </row>
-    <row r="46" spans="1:33">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -2763,7 +2291,7 @@
       <c r="AF46" s="1"/>
       <c r="AG46" s="1"/>
     </row>
-    <row r="47" spans="1:33">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -2798,7 +2326,7 @@
       <c r="AF47" s="1"/>
       <c r="AG47" s="1"/>
     </row>
-    <row r="48" spans="1:33">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -2833,7 +2361,7 @@
       <c r="AF48" s="1"/>
       <c r="AG48" s="1"/>
     </row>
-    <row r="49" spans="1:33">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -2868,7 +2396,7 @@
       <c r="AF49" s="1"/>
       <c r="AG49" s="1"/>
     </row>
-    <row r="50" spans="1:33">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -2903,7 +2431,7 @@
       <c r="AF50" s="1"/>
       <c r="AG50" s="1"/>
     </row>
-    <row r="51" spans="1:33">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2938,7 +2466,7 @@
       <c r="AF51" s="1"/>
       <c r="AG51" s="1"/>
     </row>
-    <row r="52" spans="1:33">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -2973,7 +2501,7 @@
       <c r="AF52" s="1"/>
       <c r="AG52" s="1"/>
     </row>
-    <row r="53" spans="1:33">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -3008,7 +2536,7 @@
       <c r="AF53" s="1"/>
       <c r="AG53" s="1"/>
     </row>
-    <row r="54" spans="1:33">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -3043,7 +2571,7 @@
       <c r="AF54" s="1"/>
       <c r="AG54" s="1"/>
     </row>
-    <row r="55" spans="1:33">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.15">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -3080,20 +2608,21 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B11:M19"/>
+    <mergeCell ref="N11:Y19"/>
+    <mergeCell ref="M4:Q4"/>
+    <mergeCell ref="B1:H2"/>
+    <mergeCell ref="B9:M10"/>
+    <mergeCell ref="N9:Y10"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="K4:L4"/>
-    <mergeCell ref="M4:O4"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:G6"/>
     <mergeCell ref="K6:M6"/>
     <mergeCell ref="N6:R6"/>
-    <mergeCell ref="B1:E2"/>
-    <mergeCell ref="B9:M10"/>
-    <mergeCell ref="N9:Y10"/>
-    <mergeCell ref="B11:M17"/>
-    <mergeCell ref="N11:Y17"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:I6"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
+  <pageSetup paperSize="9" scale="46" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>